<commit_message>
updated pcb and bom with test points
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\ECE477\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Personal\GitHub\ECE477\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="142">
   <si>
     <t>Qty</t>
   </si>
@@ -463,6 +463,18 @@
   </si>
   <si>
     <t>OLED Display + zif!!!</t>
+  </si>
+  <si>
+    <t>A106145CT-ND</t>
+  </si>
+  <si>
+    <t>Test Point</t>
+  </si>
+  <si>
+    <t>T1, T2, T3, T4, T5</t>
+  </si>
+  <si>
+    <t>Test point</t>
   </si>
 </sst>
 </file>
@@ -799,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,7 +870,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="1">
-        <f>A2*6</f>
+        <f t="shared" ref="B2:B31" si="0">A2*6</f>
         <v>36</v>
       </c>
       <c r="C2" s="1">
@@ -891,7 +903,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="1">
-        <f>A3*6</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="C3" s="1">
@@ -924,7 +936,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <f>A4*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C4" s="1">
@@ -957,7 +969,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <f>A5*6</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C5" s="1">
@@ -990,7 +1002,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <f>A6*6</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C6" s="1">
@@ -1023,7 +1035,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <f>A7*6</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C7" s="1">
@@ -1056,7 +1068,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="1">
-        <f>A8*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C8" s="1">
@@ -1089,7 +1101,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <f>A9*6</f>
+        <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="C9" s="1">
@@ -1122,7 +1134,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="1">
-        <f>A10*6</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C10" s="1">
@@ -1155,7 +1167,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="1">
-        <f>A11*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C11" s="1">
@@ -1188,7 +1200,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="1">
-        <f>A12*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C12" s="1"/>
@@ -1215,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="1">
-        <f>A13*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C13" s="1">
@@ -1248,7 +1260,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="1">
-        <f>A14*6</f>
+        <f t="shared" si="0"/>
         <v>102</v>
       </c>
       <c r="C14" s="1">
@@ -1281,7 +1293,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="1">
-        <f>A15*6</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C15" s="1">
@@ -1314,7 +1326,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="1">
-        <f>A16*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C16" s="1">
@@ -1347,7 +1359,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="1">
-        <f>A17*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C17" s="1">
@@ -1380,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="1">
-        <f>A18*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C18" s="1">
@@ -1413,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="1">
-        <f>A19*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C19" s="1">
@@ -1446,7 +1458,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="1">
-        <f>A20*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C20" s="1">
@@ -1479,7 +1491,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="1">
-        <f>A21*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C21" s="1">
@@ -1512,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="B22">
-        <f>A22*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D22" t="s">
@@ -1542,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <f>A23*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E23" t="s">
@@ -1569,7 +1581,7 @@
         <v>1</v>
       </c>
       <c r="B24">
-        <f>A24*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D24" t="s">
@@ -1599,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="1">
-        <f>A25*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C25" s="1">
@@ -1632,7 +1644,7 @@
         <v>1</v>
       </c>
       <c r="B26">
-        <f>A26*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C26">
@@ -1665,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="1">
-        <f>A27*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C27" s="1">
@@ -1698,7 +1710,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="1">
-        <f>A28*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C28" s="1">
@@ -1731,7 +1743,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="1">
-        <f>A29*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C29" s="1">
@@ -1764,7 +1776,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="1">
-        <f>A30*6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C30" s="1">
@@ -1790,6 +1802,36 @@
       </c>
       <c r="J30" s="1" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>30</v>
+      </c>
+      <c r="E31" t="s">
+        <v>139</v>
+      </c>
+      <c r="F31">
+        <v>603</v>
+      </c>
+      <c r="G31" t="s">
+        <v>140</v>
+      </c>
+      <c r="H31" t="s">
+        <v>141</v>
+      </c>
+      <c r="I31" t="s">
+        <v>91</v>
+      </c>
+      <c r="J31" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1797,6 +1839,6 @@
     <sortCondition ref="G2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding actual gerber files
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmolo/ECE477/Hardware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\GitHub\ECE477\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20460"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="20460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,13 @@
   <definedNames>
     <definedName name="SmartWatch" localSheetId="0">Sheet1!$A$1:$J$30</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -544,7 +544,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -565,11 +565,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -604,11 +599,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -898,26 +892,26 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="G16" sqref="A1:J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="68.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -949,7 +943,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>6</v>
       </c>
@@ -982,7 +976,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>8</v>
       </c>
@@ -1015,7 +1009,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -1048,7 +1042,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1081,7 +1075,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -1114,7 +1108,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -1147,7 +1141,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -1180,7 +1174,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1213,7 +1207,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1246,7 +1240,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1279,7 +1273,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -1306,7 +1300,7 @@
       </c>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -1339,7 +1333,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>17</v>
       </c>
@@ -1372,7 +1366,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -1405,7 +1399,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -1438,7 +1432,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1</v>
       </c>
@@ -1471,7 +1465,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -1504,7 +1498,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>1</v>
       </c>
@@ -1537,7 +1531,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>1</v>
       </c>
@@ -1570,7 +1564,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
@@ -1603,7 +1597,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -1634,7 +1628,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -1663,7 +1657,7 @@
         <v>2633</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -1694,7 +1688,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1</v>
       </c>
@@ -1727,7 +1721,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -1760,7 +1754,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -1793,7 +1787,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>1</v>
       </c>
@@ -1826,7 +1820,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>1</v>
       </c>
@@ -1859,7 +1853,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>1</v>
       </c>
@@ -1892,180 +1886,187 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>5</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <v>30</v>
       </c>
-      <c r="E31" t="s">
+      <c r="D31" s="1"/>
+      <c r="E31" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="1">
         <v>603</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G31" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I31" t="s">
-        <v>91</v>
-      </c>
-      <c r="J31" s="3" t="s">
+      <c r="I31" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>5</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E32" t="s">
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>3</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="D33">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1">
         <v>82</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="1">
         <v>603</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H33" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I33" t="s">
-        <v>91</v>
-      </c>
-      <c r="J33" t="s">
+      <c r="I33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J33" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>1</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="1">
         <v>603</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="I34" t="s">
-        <v>91</v>
-      </c>
-      <c r="J34" t="s">
+      <c r="I34" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J34" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>1</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="1">
         <v>603</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H35" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="I35" t="s">
-        <v>91</v>
-      </c>
-      <c r="J35" t="s">
+      <c r="I35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J35" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>1</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>603</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="I36" t="s">
-        <v>91</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="I36" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2073,7 +2074,7 @@
   <sortState ref="C2:H32">
     <sortCondition ref="G2"/>
   </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>